<commit_message>
API routes changed for EXcel Sheet.
</commit_message>
<xml_diff>
--- a/FlashCard/04_API/APi_Sheet.xlsx
+++ b/FlashCard/04_API/APi_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hussa\OneDrive\Desktop\CAPSTONE\20240319_Capstone\FlashCard\04_API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC1A71F3-64C6-4E60-AA6B-E12C410E4CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{09260641-4D5F-4E79-9B2A-B9BE7BB77556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{10847142-D3CB-4EE1-A55F-2B75872F020C}"/>
   </bookViews>
@@ -126,33 +126,21 @@
     <t>{401 : Token not Provided}, {403 : Forbidden request}, {404 : User not Found}, {500 : Failed to delete user}</t>
   </si>
   <si>
-    <t>decks/:id/upvote</t>
-  </si>
-  <si>
     <t>Upvote recorded</t>
   </si>
   <si>
     <t>{401 : Token not Provided}, {404 : Deck not Found}, {500 : Failed to upvote}</t>
   </si>
   <si>
-    <t>decks/:id/downvote</t>
-  </si>
-  <si>
     <t>Downvote recorded</t>
   </si>
   <si>
     <t>{401 : Token not Provided}, {404 : Deck not Found}, {500 : Failed to downvote}</t>
   </si>
   <si>
-    <t>flashcards/:id/upvote</t>
-  </si>
-  <si>
     <t>{401 : Token not Provided}, {404 : Flashcard not Found}, {500 : Failed to upvote}</t>
   </si>
   <si>
-    <t>flashcards/:id/downvote</t>
-  </si>
-  <si>
     <t>{401 : Token not Provided}, {404 : Flashcard not Found}, {500 : Failed to downvote}</t>
   </si>
   <si>
@@ -195,18 +183,12 @@
     <t>{401 : Token not Provided}, {403 : Forbidden request}, {404 : Flashcard not Found}, {500 : Failed to update flashcard permissions}</t>
   </si>
   <si>
-    <t>/api/flashcards</t>
-  </si>
-  <si>
     <t>List of flashcards [{flashcard_details}, ...]</t>
   </si>
   <si>
     <t>{500 : Internal Server Error}</t>
   </si>
   <si>
-    <t>/api/flashcards/:id</t>
-  </si>
-  <si>
     <t>Flashcard details {flashcard_details}</t>
   </si>
   <si>
@@ -225,15 +207,9 @@
     <t>Flashcard deleted</t>
   </si>
   <si>
-    <t>/api/decks</t>
-  </si>
-  <si>
     <t>List of decks [{deck_details}, ...]</t>
   </si>
   <si>
-    <t>/api/decks/:id</t>
-  </si>
-  <si>
     <t>Deck details {deck_details}</t>
   </si>
   <si>
@@ -268,6 +244,30 @@
   </si>
   <si>
     <t>{401 : Not authorised },{400 : Deck not Found}, {500 : Failed to delete Deck}</t>
+  </si>
+  <si>
+    <t>decksvote/:id/downvote</t>
+  </si>
+  <si>
+    <t>decksvote/:id/upvote</t>
+  </si>
+  <si>
+    <t>flashcardsvote/:id/upvote</t>
+  </si>
+  <si>
+    <t>flashcardsvote/:id/downvote</t>
+  </si>
+  <si>
+    <t>flashcards</t>
+  </si>
+  <si>
+    <t>flashcards/:id</t>
+  </si>
+  <si>
+    <t>decks</t>
+  </si>
+  <si>
+    <t>decks/:id</t>
   </si>
 </sst>
 </file>
@@ -726,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E77DEA-1122-45D9-8819-81FEED87F59D}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.6640625" defaultRowHeight="45.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -941,7 +941,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -956,10 +956,10 @@
         <v>201</v>
       </c>
       <c r="H8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -970,7 +970,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -985,10 +985,10 @@
         <v>201</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -999,7 +999,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -1014,10 +1014,10 @@
         <v>201</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1028,7 +1028,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
@@ -1043,10 +1043,10 @@
         <v>201</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1057,13 +1057,13 @@
         <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>21</v>
@@ -1072,10 +1072,10 @@
         <v>200</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1086,25 +1086,25 @@
         <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="1">
+        <v>200</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="1">
-        <v>200</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="I13" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1115,13 +1115,13 @@
         <v>27</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>21</v>
@@ -1130,10 +1130,10 @@
         <v>200</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1144,25 +1144,25 @@
         <v>27</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="1">
+        <v>200</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" s="1">
-        <v>200</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1173,7 +1173,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>11</v>
@@ -1188,10 +1188,10 @@
         <v>200</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1202,7 +1202,7 @@
         <v>19</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>11</v>
@@ -1217,10 +1217,10 @@
         <v>200</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1231,13 +1231,13 @@
         <v>9</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>21</v>
@@ -1246,10 +1246,10 @@
         <v>201</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1260,13 +1260,13 @@
         <v>27</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>21</v>
@@ -1275,10 +1275,10 @@
         <v>200</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1289,25 +1289,25 @@
         <v>30</v>
       </c>
       <c r="C20" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="5">
+        <v>200</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="5">
-        <v>200</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="I20" s="6" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1318,7 +1318,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>11</v>
@@ -1333,10 +1333,10 @@
         <v>200</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1347,7 +1347,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>11</v>
@@ -1362,10 +1362,10 @@
         <v>200</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1376,13 +1376,13 @@
         <v>9</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>21</v>
@@ -1391,10 +1391,10 @@
         <v>201</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1405,25 +1405,25 @@
         <v>27</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="7">
+        <v>200</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="I24" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24" s="7">
-        <v>200</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="I24" s="8" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1434,7 +1434,7 @@
         <v>30</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>11</v>
@@ -1449,10 +1449,10 @@
         <v>200</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding User and Auth APIs
</commit_message>
<xml_diff>
--- a/FlashCard/04_API/APi_Sheet.xlsx
+++ b/FlashCard/04_API/APi_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hussa\OneDrive\Desktop\CAPSTONE\20240319_Capstone\FlashCard\04_API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09260641-4D5F-4E79-9B2A-B9BE7BB77556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74531700-F8AE-48A1-B71A-98A25B258190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{10847142-D3CB-4EE1-A55F-2B75872F020C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="83">
   <si>
     <t>S.No</t>
   </si>
@@ -96,12 +96,6 @@
     <t>User logged out</t>
   </si>
   <si>
-    <t>users/:id</t>
-  </si>
-  <si>
-    <t>id : …....</t>
-  </si>
-  <si>
     <t>User details {user_details}</t>
   </si>
   <si>
@@ -268,6 +262,18 @@
   </si>
   <si>
     <t>decks/:id</t>
+  </si>
+  <si>
+    <t>decks/post</t>
+  </si>
+  <si>
+    <t>users/getdetails</t>
+  </si>
+  <si>
+    <t>users/update/:id</t>
+  </si>
+  <si>
+    <t>users/delete/:id</t>
   </si>
 </sst>
 </file>
@@ -726,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E77DEA-1122-45D9-8819-81FEED87F59D}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.6640625" defaultRowHeight="45.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -854,25 +860,23 @@
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="1">
+        <v>200</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="I5" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="1">
-        <v>200</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -880,10 +884,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -898,10 +902,10 @@
         <v>200</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -909,28 +913,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="1">
+        <v>200</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="1">
-        <v>200</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -941,7 +945,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -956,10 +960,10 @@
         <v>201</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -970,7 +974,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -985,10 +989,10 @@
         <v>201</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -999,7 +1003,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -1014,10 +1018,10 @@
         <v>201</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1028,7 +1032,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
@@ -1043,10 +1047,10 @@
         <v>201</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1054,28 +1058,28 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="1">
+        <v>200</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="I12" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="1">
-        <v>200</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1083,28 +1087,28 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="1">
+        <v>200</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="1">
-        <v>200</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1112,28 +1116,28 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="1">
+        <v>200</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="I14" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="1">
-        <v>200</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1141,16 +1145,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>21</v>
@@ -1159,10 +1163,10 @@
         <v>200</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1173,7 +1177,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>11</v>
@@ -1188,10 +1192,10 @@
         <v>200</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1202,7 +1206,7 @@
         <v>19</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>11</v>
@@ -1217,10 +1221,10 @@
         <v>200</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1231,13 +1235,13 @@
         <v>9</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>21</v>
@@ -1246,10 +1250,10 @@
         <v>201</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1257,16 +1261,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>11</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>21</v>
@@ -1275,10 +1279,10 @@
         <v>200</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1286,10 +1290,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>11</v>
@@ -1304,10 +1308,10 @@
         <v>200</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1318,7 +1322,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>11</v>
@@ -1333,10 +1337,10 @@
         <v>200</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1347,7 +1351,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>11</v>
@@ -1362,10 +1366,10 @@
         <v>200</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1382,7 +1386,7 @@
         <v>11</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>21</v>
@@ -1391,10 +1395,10 @@
         <v>201</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1402,16 +1406,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>11</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F24" s="7" t="s">
         <v>21</v>
@@ -1420,10 +1424,10 @@
         <v>200</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1431,10 +1435,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>11</v>
@@ -1449,10 +1453,10 @@
         <v>200</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deck CRUD API added and API sheet update for it.
</commit_message>
<xml_diff>
--- a/FlashCard/04_API/APi_Sheet.xlsx
+++ b/FlashCard/04_API/APi_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hussa\OneDrive\Desktop\CAPSTONE\20240319_Capstone\FlashCard\04_API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74531700-F8AE-48A1-B71A-98A25B258190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27079EDB-5AFF-40F7-9333-27CCD91A8E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{10847142-D3CB-4EE1-A55F-2B75872F020C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="85">
   <si>
     <t>S.No</t>
   </si>
@@ -258,12 +258,6 @@
     <t>flashcards/:id</t>
   </si>
   <si>
-    <t>decks</t>
-  </si>
-  <si>
-    <t>decks/:id</t>
-  </si>
-  <si>
     <t>decks/post</t>
   </si>
   <si>
@@ -274,6 +268,18 @@
   </si>
   <si>
     <t>users/delete/:id</t>
+  </si>
+  <si>
+    <t>decks/getAll</t>
+  </si>
+  <si>
+    <t>decks/get/:id</t>
+  </si>
+  <si>
+    <t>decks/update/:id</t>
+  </si>
+  <si>
+    <t>decks/delete/:id</t>
   </si>
 </sst>
 </file>
@@ -732,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E77DEA-1122-45D9-8819-81FEED87F59D}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.6640625" defaultRowHeight="45.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -860,7 +866,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
@@ -887,7 +893,7 @@
         <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -916,7 +922,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -1322,7 +1328,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>11</v>
@@ -1351,7 +1357,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>11</v>
@@ -1380,7 +1386,7 @@
         <v>9</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>11</v>
@@ -1409,7 +1415,7 @@
         <v>25</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>11</v>
@@ -1438,7 +1444,7 @@
         <v>28</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Create API for Flashcard and API sheet updated for it.
</commit_message>
<xml_diff>
--- a/FlashCard/04_API/APi_Sheet.xlsx
+++ b/FlashCard/04_API/APi_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hussa\OneDrive\Desktop\CAPSTONE\20240319_Capstone\FlashCard\04_API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27079EDB-5AFF-40F7-9333-27CCD91A8E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4E2254-1A5F-4EF5-9215-4A34DA764A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{10847142-D3CB-4EE1-A55F-2B75872F020C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="88">
   <si>
     <t>S.No</t>
   </si>
@@ -252,12 +252,6 @@
     <t>flashcardsvote/:id/downvote</t>
   </si>
   <si>
-    <t>flashcards</t>
-  </si>
-  <si>
-    <t>flashcards/:id</t>
-  </si>
-  <si>
     <t>decks/post</t>
   </si>
   <si>
@@ -280,6 +274,21 @@
   </si>
   <si>
     <t>decks/delete/:id</t>
+  </si>
+  <si>
+    <t>flashcards/getAll</t>
+  </si>
+  <si>
+    <t>flashcards/get/:id</t>
+  </si>
+  <si>
+    <t>flashcards/:deckId</t>
+  </si>
+  <si>
+    <t>flashcards/update/:deckId</t>
+  </si>
+  <si>
+    <t>flashcards/delete/:deckid</t>
   </si>
 </sst>
 </file>
@@ -738,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E77DEA-1122-45D9-8819-81FEED87F59D}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.6640625" defaultRowHeight="45.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -866,7 +875,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
@@ -893,7 +902,7 @@
         <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -922,7 +931,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -1183,7 +1192,7 @@
         <v>19</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>11</v>
@@ -1212,7 +1221,7 @@
         <v>19</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>11</v>
@@ -1241,7 +1250,7 @@
         <v>9</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>11</v>
@@ -1270,7 +1279,7 @@
         <v>25</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>11</v>
@@ -1299,7 +1308,7 @@
         <v>28</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>11</v>
@@ -1328,7 +1337,7 @@
         <v>19</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>11</v>
@@ -1357,7 +1366,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>11</v>
@@ -1386,7 +1395,7 @@
         <v>9</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>11</v>
@@ -1415,7 +1424,7 @@
         <v>25</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>11</v>
@@ -1444,7 +1453,7 @@
         <v>28</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
API sheet updated and Voting API created.
</commit_message>
<xml_diff>
--- a/FlashCard/04_API/APi_Sheet.xlsx
+++ b/FlashCard/04_API/APi_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hussa\OneDrive\Desktop\CAPSTONE\20240319_Capstone\FlashCard\04_API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4E2254-1A5F-4EF5-9215-4A34DA764A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5930E460-A44F-4CCB-BB12-EDC34E7E792C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{10847142-D3CB-4EE1-A55F-2B75872F020C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="79">
   <si>
     <t>S.No</t>
   </si>
@@ -138,45 +138,6 @@
     <t>{401 : Token not Provided}, {404 : Flashcard not Found}, {500 : Failed to downvote}</t>
   </si>
   <si>
-    <t>decks/:id/visibility</t>
-  </si>
-  <si>
-    <t>{ "visibility": "public" }</t>
-  </si>
-  <si>
-    <t>Deck visibility updated</t>
-  </si>
-  <si>
-    <t>{401 : Token not Provided}, {403 : Forbidden request}, {404 : Deck not Found}, {500 : Failed to update deck visibility}</t>
-  </si>
-  <si>
-    <t>flashcards/:id/visibility</t>
-  </si>
-  <si>
-    <t>Flashcard visibility updated</t>
-  </si>
-  <si>
-    <t>{401 : Token not Provided}, {403 : Forbidden request}, {404 : Flashcard not Found}, {500 : Failed to update flashcard visibility}</t>
-  </si>
-  <si>
-    <t>decks/:id/permissions</t>
-  </si>
-  <si>
-    <t>{ "userId": "...", "permissionLevel": "edit" }</t>
-  </si>
-  <si>
-    <t>Permissions updated</t>
-  </si>
-  <si>
-    <t>{401 : Token not Provided}, {403 : Forbidden request}, {404 : Deck not Found}, {500 : Failed to update deck permissions}</t>
-  </si>
-  <si>
-    <t>flashcards/:id/permissions</t>
-  </si>
-  <si>
-    <t>{401 : Token not Provided}, {403 : Forbidden request}, {404 : Flashcard not Found}, {500 : Failed to update flashcard permissions}</t>
-  </si>
-  <si>
     <t>List of flashcards [{flashcard_details}, ...]</t>
   </si>
   <si>
@@ -289,6 +250,18 @@
   </si>
   <si>
     <t>flashcards/delete/:deckid</t>
+  </si>
+  <si>
+    <t>{ "query": "string" }</t>
+  </si>
+  <si>
+    <t>{ "results": [...] }</t>
+  </si>
+  <si>
+    <t>/search/q</t>
+  </si>
+  <si>
+    <t>{ 500  : Failed to perform search }</t>
   </si>
 </sst>
 </file>
@@ -341,7 +314,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -401,11 +374,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE3E3E3"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -429,6 +411,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -745,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4E77DEA-1122-45D9-8819-81FEED87F59D}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.6640625" defaultRowHeight="45.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -875,7 +860,7 @@
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
@@ -902,7 +887,7 @@
         <v>25</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>11</v>
@@ -931,7 +916,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>11</v>
@@ -960,7 +945,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
@@ -989,7 +974,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>11</v>
@@ -1018,7 +1003,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
@@ -1047,7 +1032,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
@@ -1072,116 +1057,116 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="5">
+        <v>200</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="I12" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="1">
-        <v>200</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="1">
+      <c r="B13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="5">
         <v>200</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>43</v>
+      <c r="H13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="1">
-        <v>200</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>47</v>
+      <c r="B14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="5">
+        <v>201</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" s="1">
+      <c r="C15" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="5">
         <v>200</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>49</v>
+      <c r="H15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1189,10 +1174,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>11</v>
@@ -1207,126 +1192,126 @@
         <v>200</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17" s="5">
+      <c r="C17" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="7">
         <v>200</v>
       </c>
-      <c r="H17" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>53</v>
+      <c r="H17" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G18" s="5">
-        <v>201</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>55</v>
+      <c r="B18" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="7">
+        <v>200</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G19" s="5">
-        <v>200</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>67</v>
+      <c r="B19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="7">
+        <v>201</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="5">
+      <c r="B20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="7">
         <v>200</v>
       </c>
-      <c r="H20" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>68</v>
+      <c r="H20" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -1334,10 +1319,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>11</v>
@@ -1352,126 +1337,39 @@
         <v>200</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G22" s="7">
+      <c r="A22" s="9">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="5">
         <v>200</v>
       </c>
-      <c r="H22" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G23" s="7">
-        <v>201</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G24" s="7">
-        <v>200</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="I24" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="45.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G25" s="7">
-        <v>200</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>70</v>
+      <c r="H22" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>